<commit_message>
Final commit, project is prensented
</commit_message>
<xml_diff>
--- a/database/expenses.xlsx
+++ b/database/expenses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,92 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>241114</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>snacks</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>120</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Chips</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>241114</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>subcriptions</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>233</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>241001</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>bills</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Electrical bill</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>241114</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>snacks</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Chips</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>